<commit_message>
Se elimina el segundo nombre y se deja una columna solo con Nombre para que el usuario escriba los nombres que tenga, pudiendo ser más de uno. Adicionalmente se agregan algunas locaciones de texto faltantes en el módulo de gestión de talento
</commit_message>
<xml_diff>
--- a/ERPSEI/wwwroot/templates/PlantillaEmpleados.xlsx
+++ b/ERPSEI/wwwroot/templates/PlantillaEmpleados.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luis_\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\luis_\source\repos\ERPSEI\ERPSEI\wwwroot\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE0597ED-3781-4240-B501-7EC4A0BBE7D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{934AF401-BF79-44EC-8DF0-0629A34FD6D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{5DC0EDEE-1DD5-4E9D-83BE-13919088A125}"/>
   </bookViews>
@@ -20,6 +20,7 @@
     <sheet name="Subareas" sheetId="11" r:id="rId5"/>
     <sheet name="Generos" sheetId="12" r:id="rId6"/>
     <sheet name="EstadosCiviles" sheetId="13" r:id="rId7"/>
+    <sheet name="Jefes" sheetId="14" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
     <author>Luis Linares</author>
   </authors>
   <commentList>
-    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{303AD3EE-C2C0-4C54-A463-2AABC3C96DBA}">
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{303AD3EE-C2C0-4C54-A463-2AABC3C96DBA}">
       <text>
         <r>
           <rPr>
@@ -120,7 +121,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{C7D42264-61F4-49DC-857C-5E45611B4A6A}">
+    <comment ref="E1" authorId="0" shapeId="0" xr:uid="{C7D42264-61F4-49DC-857C-5E45611B4A6A}">
       <text>
         <r>
           <rPr>
@@ -164,7 +165,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{7F806EAD-B0D5-4174-819E-6FB84BCBA105}">
+    <comment ref="F1" authorId="0" shapeId="0" xr:uid="{7F806EAD-B0D5-4174-819E-6FB84BCBA105}">
       <text>
         <r>
           <rPr>
@@ -181,14 +182,14 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t xml:space="preserve">
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{179D3CB5-70FE-46BB-8EE6-FD8FC25DDA7E}">
+    <comment ref="G1" authorId="0" shapeId="0" xr:uid="{179D3CB5-70FE-46BB-8EE6-FD8FC25DDA7E}">
       <text>
         <r>
           <rPr>
@@ -212,7 +213,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{0A89D469-7E79-4978-A7D6-994178A3BFFF}">
+    <comment ref="I1" authorId="0" shapeId="0" xr:uid="{0A89D469-7E79-4978-A7D6-994178A3BFFF}">
       <text>
         <r>
           <rPr>
@@ -236,7 +237,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{3B34D01C-E41F-4985-8BB0-C6756BD3DCD3}">
+    <comment ref="J1" authorId="0" shapeId="0" xr:uid="{3B34D01C-E41F-4985-8BB0-C6756BD3DCD3}">
       <text>
         <r>
           <rPr>
@@ -250,7 +251,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{7C1F3399-CD2D-4A1C-BEFE-F0C801F7E9B8}">
+    <comment ref="K1" authorId="0" shapeId="0" xr:uid="{7C1F3399-CD2D-4A1C-BEFE-F0C801F7E9B8}">
       <text>
         <r>
           <rPr>
@@ -274,7 +275,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0" xr:uid="{DC304CE0-1838-4456-BE40-51A72511ACA9}">
+    <comment ref="L1" authorId="0" shapeId="0" xr:uid="{DC304CE0-1838-4456-BE40-51A72511ACA9}">
       <text>
         <r>
           <rPr>
@@ -288,7 +289,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{EB242D86-D769-4D0D-B083-F65C3B995008}">
+    <comment ref="N1" authorId="0" shapeId="0" xr:uid="{EFFE5E71-41FD-455D-A810-2560627F1525}">
       <text>
         <r>
           <rPr>
@@ -298,119 +299,95 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Nombre completo del Jefe, empezando por el nombre y luego los apellidos.</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
+          <t xml:space="preserve">Formato esperado:
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">yyyy-mm-dd
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>yyyy:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> año a cuatro dígitos
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>mm:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> mes a dos dígitos
+</t>
+        </r>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>dd:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve"> día a dos dígitos
 </t>
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0" shapeId="0" xr:uid="{EFFE5E71-41FD-455D-A810-2560627F1525}">
+    <comment ref="P1" authorId="0" shapeId="0" xr:uid="{328AFE3A-A373-4932-8F42-6B2C6B7EE120}">
       <text>
         <r>
           <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">Formato esperado:
-</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">yyyy-mm-dd
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>yyyy:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> año a cuatro dígitos
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>mm:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> mes a dos dígitos
-</t>
-        </r>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>dd:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve"> día a dos dígitos
-</t>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nombre completo empezando por el nombre.</t>
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0" shapeId="0" xr:uid="{328AFE3A-A373-4932-8F42-6B2C6B7EE120}">
-      <text>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Nombre completo empezando por el nombre.</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="S1" authorId="0" shapeId="0" xr:uid="{495A2CA3-CF18-4201-9822-5DD20431C6D2}">
+    <comment ref="R1" authorId="0" shapeId="0" xr:uid="{495A2CA3-CF18-4201-9822-5DD20431C6D2}">
       <text>
         <r>
           <rPr>
@@ -429,7 +406,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="122">
   <si>
     <t>APELLIDO PATERNO</t>
   </si>
@@ -467,12 +444,6 @@
     <t>FECHA NACIMIENTO</t>
   </si>
   <si>
-    <t>PRIMER NOMBRE</t>
-  </si>
-  <si>
-    <t>SEGUNDO NOMBRE</t>
-  </si>
-  <si>
     <t>TELÉFONO</t>
   </si>
   <si>
@@ -675,6 +646,132 @@
   </si>
   <si>
     <t>Soltero</t>
+  </si>
+  <si>
+    <t>NOMBRE(S)</t>
+  </si>
+  <si>
+    <t>Grupo</t>
+  </si>
+  <si>
+    <t>Edgar Cruz Antonio</t>
+  </si>
+  <si>
+    <t>Carlos Alberto Díaz Silveti Camargo</t>
+  </si>
+  <si>
+    <t>César Dondiego Martínez</t>
+  </si>
+  <si>
+    <t>Iván Linares Hernández</t>
+  </si>
+  <si>
+    <t>Antonio Lomelí de la Torre</t>
+  </si>
+  <si>
+    <t>Nelly Guadalupe López Villalobos</t>
+  </si>
+  <si>
+    <t>Clarisa María Verónica Magaña Bou</t>
+  </si>
+  <si>
+    <t>Ana Silvia Martínez Hernández</t>
+  </si>
+  <si>
+    <t>Julio César Romero Navarrete</t>
+  </si>
+  <si>
+    <t>Marco Cabrera Daniel</t>
+  </si>
+  <si>
+    <t>Laura Aldana Nieto</t>
+  </si>
+  <si>
+    <t>Jesús Martín Blanco Nilo</t>
+  </si>
+  <si>
+    <t>Noé Coca Anaya</t>
+  </si>
+  <si>
+    <t>Tania Cruz Cruz</t>
+  </si>
+  <si>
+    <t>Guillermo Díaz Bermúdez</t>
+  </si>
+  <si>
+    <t>José Martín Díaz Juárez</t>
+  </si>
+  <si>
+    <t>Verónica Fernández Reyes</t>
+  </si>
+  <si>
+    <t>Alfredo Iván Flores Aranda</t>
+  </si>
+  <si>
+    <t>Samantha Skarlet Gómez Jiménez</t>
+  </si>
+  <si>
+    <t>Alejandro Hernández Esquivel</t>
+  </si>
+  <si>
+    <t>César Augusto Maldonado Aguilar</t>
+  </si>
+  <si>
+    <t>José Luis Ortega Alcántara</t>
+  </si>
+  <si>
+    <t>Yonir Santos Pinacho</t>
+  </si>
+  <si>
+    <t>Hiran Gabriel Torres López</t>
+  </si>
+  <si>
+    <t>Itzchell Vera Aguilar</t>
+  </si>
+  <si>
+    <t>Nancy Bautista Hipólito</t>
+  </si>
+  <si>
+    <t>Mitzy Sharai Cedillo Mayén</t>
+  </si>
+  <si>
+    <t>Yolanda Delgado Rivera</t>
+  </si>
+  <si>
+    <t>Rodolfo Doroteo Cortez</t>
+  </si>
+  <si>
+    <t>Sergio Carlos Hernández Nolasco</t>
+  </si>
+  <si>
+    <t>Guadalupe Esmeralda Martínez Rodríguez</t>
+  </si>
+  <si>
+    <t>Enrique Morales Bernal</t>
+  </si>
+  <si>
+    <t>Joseph Iván Moreno Barrios</t>
+  </si>
+  <si>
+    <t>Raymundo Quintos Paredes</t>
+  </si>
+  <si>
+    <t>Ismael Anderik Ramírez Borja</t>
+  </si>
+  <si>
+    <t>Alejandro Arturo González Martín</t>
+  </si>
+  <si>
+    <t>Francisco Méndez</t>
+  </si>
+  <si>
+    <t>Ramón Alberto Prado Cruz</t>
+  </si>
+  <si>
+    <t>Ángel</t>
+  </si>
+  <si>
+    <t>Juán Aldasoro</t>
   </si>
 </sst>
 </file>
@@ -684,7 +781,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -743,14 +840,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -769,8 +860,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -793,12 +908,25 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -817,6 +945,25 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1143,121 +1290,116 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="136.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="17" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="43.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="27.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="43.7109375" style="2" customWidth="1"/>
-    <col min="18" max="18" width="22.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="43.7109375" style="2" customWidth="1"/>
-    <col min="20" max="20" width="22.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="23" width="30.7109375" style="2" customWidth="1"/>
+    <col min="1" max="1" width="36.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="136.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="17" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="43.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15" style="3" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="27.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="43.7109375" style="2" customWidth="1"/>
+    <col min="17" max="17" width="22.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="43.7109375" style="2" customWidth="1"/>
+    <col min="19" max="19" width="22.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="22" width="30.7109375" style="2" customWidth="1"/>
+    <col min="23" max="23" width="0" hidden="1" customWidth="1"/>
     <col min="24" max="16384" width="11.42578125" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:22" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L1" s="1" t="s">
+      <c r="P1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="Q1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>22</v>
-      </c>
       <c r="T1" s="1" t="s">
-        <v>20</v>
+        <v>4</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="W1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="E2" s="3"/>
-      <c r="I2" s="6"/>
-      <c r="N2" s="4"/>
-      <c r="O2" s="3"/>
-      <c r="P2" s="5"/>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25"/>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="H2" s="6"/>
+      <c r="M2" s="4"/>
+      <c r="O2" s="5"/>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25"/>
     <row r="17" x14ac:dyDescent="0.25"/>
     <row r="18" x14ac:dyDescent="0.25"/>
     <row r="19" x14ac:dyDescent="0.25"/>
@@ -1398,40 +1540,46 @@
   <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="6">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{87877414-FB8C-4177-B26F-0D85E2FD1114}">
           <x14:formula1>
             <xm:f>Generos!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>G3:G1048576 G2</xm:sqref>
+          <xm:sqref>F2:F1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{ADCB6A4C-97F7-4104-A127-9B7CA99311CD}">
           <x14:formula1>
             <xm:f>EstadosCiviles!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H1048576</xm:sqref>
+          <xm:sqref>G2:G1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{ADA7C5EA-D192-4838-AA3F-184B29E7C2A4}">
           <x14:formula1>
             <xm:f>Puestos!$B$2:$B$19</xm:f>
           </x14:formula1>
-          <xm:sqref>J2:J1048576</xm:sqref>
+          <xm:sqref>I2:I1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F6E37C78-A1F2-468B-A6F7-AB2DA566F158}">
           <x14:formula1>
             <xm:f>Áreas!$B$2:$B$15</xm:f>
           </x14:formula1>
-          <xm:sqref>K2:K1048576</xm:sqref>
+          <xm:sqref>J2:J1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{696301D3-A781-4A87-BE9A-CE08E6478DB7}">
           <x14:formula1>
             <xm:f>Subareas!$B$2:$B$9</xm:f>
           </x14:formula1>
-          <xm:sqref>L2:L1048576</xm:sqref>
+          <xm:sqref>K2:K1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DB18B4DA-A24B-41B7-AB54-84236CDB8B86}">
           <x14:formula1>
             <xm:f>Oficinas!$B$2:$B$15</xm:f>
+          </x14:formula1>
+          <xm:sqref>L2:L1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{DCE21C94-1B59-4923-BD24-5A67CA1C5191}">
+          <x14:formula1>
+            <xm:f>Jefes!$B$2:$B$41</xm:f>
           </x14:formula1>
           <xm:sqref>M2:M1048576</xm:sqref>
         </x14:dataValidation>
@@ -1456,10 +1604,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1467,7 +1615,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1475,7 +1623,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1483,7 +1631,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1491,7 +1639,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1499,7 +1647,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1507,7 +1655,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1515,7 +1663,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1523,7 +1671,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1531,7 +1679,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1539,7 +1687,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1547,7 +1695,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1555,7 +1703,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -1563,7 +1711,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -1571,7 +1719,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1594,10 +1742,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1605,7 +1753,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1613,7 +1761,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1621,7 +1769,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1629,7 +1777,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1637,7 +1785,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1645,7 +1793,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1653,7 +1801,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1661,7 +1809,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1669,7 +1817,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1677,7 +1825,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1685,7 +1833,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1693,7 +1841,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -1701,7 +1849,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -1709,7 +1857,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -1717,7 +1865,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -1725,7 +1873,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -1733,7 +1881,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1741,7 +1889,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1764,10 +1912,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1775,7 +1923,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1783,7 +1931,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1791,7 +1939,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1799,7 +1947,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1807,7 +1955,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1815,7 +1963,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1823,7 +1971,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1831,7 +1979,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1839,7 +1987,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -1847,7 +1995,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -1855,7 +2003,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -1863,7 +2011,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -1871,7 +2019,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -1879,7 +2027,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1902,10 +2050,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1913,7 +2061,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1921,7 +2069,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1929,7 +2077,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1937,7 +2085,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1945,7 +2093,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1953,7 +2101,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1961,7 +2109,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -1969,7 +2117,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -1989,10 +2137,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2000,7 +2148,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2008,7 +2156,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
   </sheetData>
@@ -2028,10 +2176,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -2039,7 +2187,7 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -2047,10 +2195,415 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E85DE1B-826A-45F4-AC60-4ECBB8CAD5E6}">
+  <dimension ref="A1:C41"/>
+  <sheetViews>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="9">
+        <v>1</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="C2" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="9">
+        <v>2</v>
+      </c>
+      <c r="B3" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="C3" s="13"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="9">
+        <v>3</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="C4" s="13"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="9">
+        <v>4</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="C5" s="13"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="10">
+        <v>5</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="C6" s="14">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="10">
+        <v>6</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C7" s="14"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="10">
+        <v>7</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" s="14"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="10">
+        <v>8</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" s="14"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="C10" s="14"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="10">
+        <v>10</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="C11" s="14"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="10">
+        <v>11</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C12" s="14"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="10">
+        <v>12</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="C13" s="14"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="10">
+        <v>13</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="C14" s="14"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="10">
+        <v>14</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C15" s="14"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="10">
+        <v>15</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="C16" s="14"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="11">
+        <v>16</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="C17" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="11">
+        <v>17</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="C18" s="15"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="11">
+        <v>18</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="C19" s="15"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="11">
+        <v>19</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20" s="15"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="11">
+        <v>20</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="C21" s="15"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="11">
+        <v>21</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="C22" s="15"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="11">
+        <v>22</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="C23" s="15"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="11">
+        <v>23</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C24" s="15"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="11">
+        <v>24</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C25" s="15"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="11">
+        <v>25</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="C26" s="15"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="11">
+        <v>26</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="C27" s="15"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="11">
+        <v>27</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="C28" s="15"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="11">
+        <v>28</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="C29" s="15"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="11">
+        <v>29</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="C30" s="15"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="11">
+        <v>30</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="C31" s="15"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="12">
+        <v>31</v>
+      </c>
+      <c r="B32" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="C32" s="16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="12">
+        <v>32</v>
+      </c>
+      <c r="B33" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="C33" s="16"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="12">
+        <v>33</v>
+      </c>
+      <c r="B34" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="C34" s="16"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="12">
+        <v>34</v>
+      </c>
+      <c r="B35" s="12" t="s">
+        <v>110</v>
+      </c>
+      <c r="C35" s="16"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="12">
+        <v>35</v>
+      </c>
+      <c r="B36" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C36" s="16"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="12">
+        <v>36</v>
+      </c>
+      <c r="B37" s="12" t="s">
+        <v>112</v>
+      </c>
+      <c r="C37" s="16"/>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="12">
+        <v>37</v>
+      </c>
+      <c r="B38" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="C38" s="16"/>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="12">
+        <v>38</v>
+      </c>
+      <c r="B39" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="C39" s="16"/>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="12">
+        <v>39</v>
+      </c>
+      <c r="B40" s="12" t="s">
+        <v>115</v>
+      </c>
+      <c r="C40" s="16"/>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="12">
+        <v>40</v>
+      </c>
+      <c r="B41" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="C41" s="16"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="C2:C5"/>
+    <mergeCell ref="C6:C16"/>
+    <mergeCell ref="C17:C31"/>
+    <mergeCell ref="C32:C41"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>